<commit_message>
-- add using today's date as the statement date
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8AEDFE-4CED-4E8C-9CBD-96C93F55DC5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="3420" yWindow="1755" windowWidth="18000" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -69,22 +70,22 @@
     <t>STATEMENT_DATE</t>
   </si>
   <si>
-    <t>C:\Users\HP\Downloads\BotFiles\</t>
-  </si>
-  <si>
-    <t>Nostro Reco Report 28th Oct 2022.xlsx</t>
-  </si>
-  <si>
-    <t>Nostro Reco Report 31st Oct 2022_.xlsx</t>
-  </si>
-  <si>
-    <t>31 OCT 2022</t>
+    <t>27 OCT 2022</t>
+  </si>
+  <si>
+    <t>NOSTRO RECO 26TH OCT 2022.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\RPA\Desktop\TestFolder\</t>
+  </si>
+  <si>
+    <t>Nostro Reco Report 27th Oct 2022_.xlsx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -114,9 +115,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -398,11 +397,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,7 +426,7 @@
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -435,49 +434,48 @@
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2" t="s">
+      <c r="C3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>14</v>
       </c>
       <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" t="s">
         <v>7</v>
       </c>
     </row>
@@ -485,8 +483,8 @@
       <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>19</v>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Mail List 21/03/23. Maximising all the windows
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8AEDFE-4CED-4E8C-9CBD-96C93F55DC5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB227D1-49F3-4D70-916B-FA082F255FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="1755" windowWidth="18000" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="12195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>KEY</t>
   </si>
@@ -70,26 +70,25 @@
     <t>STATEMENT_DATE</t>
   </si>
   <si>
-    <t>27 OCT 2022</t>
-  </si>
-  <si>
-    <t>NOSTRO RECO 26TH OCT 2022.xlsx</t>
-  </si>
-  <si>
-    <t>C:\Users\RPA\Desktop\TestFolder\</t>
-  </si>
-  <si>
-    <t>Nostro Reco Report 27th Oct 2022_.xlsx</t>
+    <t>\\10.222.140.144\d\d\MIS\GLS\RPA_BOT\</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -112,14 +111,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -401,7 +403,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,9 +444,6 @@
       <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
       <c r="C4" t="s">
         <v>3</v>
       </c>
@@ -453,9 +452,6 @@
       <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
       <c r="C5" t="s">
         <v>4</v>
       </c>
@@ -472,8 +468,8 @@
       <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
-        <v>18</v>
+      <c r="B7" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
@@ -483,12 +479,13 @@
       <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="B8" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{6A4F96ED-FF18-43C0-AD29-F7F07FBF2315}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>